<commit_message>
Downloaded updated versions of focus city bond data
</commit_message>
<xml_diff>
--- a/DATA/RAW/bond_data/os_PA3060059_ReadingArea.xlsx
+++ b/DATA/RAW/bond_data/os_PA3060059_ReadingArea.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walke\AppData\Local\Box\Box Edit\Documents\9HA8m6f8+0aDAm0uSCUxLw==\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walke\OneDrive\Documents\Duke\Masters Project\Shrinking_Cities_MP\DATA\RAW\bond_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C98B283-EA37-4B3A-8C36-55803D1253FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673845D1-DA10-445B-81FE-4CCCFDD1AC20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2230" yWindow="1300" windowWidth="14400" windowHeight="7360" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -1977,7 +1977,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2067,13 +2067,138 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2084,6 +2209,35 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1E97BD8-BC68-4576-AA8D-B3F5F54033C6}" name="Table1" displayName="Table1" ref="A1:J29" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="12">
+  <autoFilter ref="A1:J29" xr:uid="{106DC70F-B2D0-4416-8EC6-A86A892CFB4A}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Industrial"/>
+        <filter val="Total"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:J29">
+    <sortCondition ref="H1:H29"/>
+  </sortState>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{A1A14B96-B51D-4C93-9D6B-0E507C9CED69}" name="PWSID" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{058943CB-E19B-41F7-A552-66F137C8CCCB}" name="name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{49F8B26E-A353-4DC1-8477-A5EB25AF9EF9}" name="OSYear" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{254B3242-7E78-4259-AB03-7054EE578E92}" name="WaterSewer" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{DE882A07-88A0-423B-A658-758A2E1956EB}" name="groupBy" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{BA26D300-0A38-4225-B9F8-2ADD1978D1A0}" name="class" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{4D16EAED-F22B-4160-8E13-8FAB97249227}" name="tier" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{FBC7A34F-2AA7-48E1-B181-A04EFCFC5BD0}" name="year" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{1E602258-952B-43B3-AF48-3E8CDF99A21D}" name="nConnections" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{20D0E895-88AC-4955-8873-D07664E70ECA}" name="notes" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4097,862 +4251,898 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.90625" style="1"/>
+    <col min="2" max="3" width="8.90625" style="1"/>
+    <col min="4" max="4" width="13.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="8.90625" style="1"/>
+    <col min="9" max="9" width="14.26953125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="50" t="s">
         <v>408</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="49" t="s">
         <v>407</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="50" t="s">
         <v>385</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="50" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" s="1">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="51">
         <v>1997</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="G2" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="51">
         <v>1997</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="51">
         <v>25672</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="J2" s="51"/>
+    </row>
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="51">
         <v>1997</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="G3" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="51">
         <v>1997</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="51">
         <v>2204</v>
       </c>
+      <c r="J3" s="51"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="A4" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="51">
         <v>1997</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="G4" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="51">
         <v>1997</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="51">
         <v>184</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="J4" s="51"/>
+    </row>
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="51">
         <v>1997</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="G5" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="51">
         <v>1997</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="51">
         <v>154</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="J5" s="51"/>
+    </row>
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="51">
         <v>1997</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="G6" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="51">
         <v>1997</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="51">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="J6" s="51"/>
+    </row>
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="51">
         <v>1997</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" s="1">
+      <c r="G7" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="51">
         <v>1997</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="51">
         <v>310</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="J7" s="51"/>
+    </row>
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="51">
         <v>2002</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="G8" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="51">
         <v>2002</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="51">
         <v>25488</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="J8" s="51"/>
+    </row>
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="51">
         <v>2002</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="G9" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" s="51">
         <v>2002</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="51">
         <v>2207</v>
       </c>
+      <c r="J9" s="51"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="A10" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="51">
         <v>2002</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H10" s="1">
+      <c r="G10" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="51">
         <v>2002</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="51">
         <v>173</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="J10" s="51"/>
+    </row>
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="51">
         <v>2002</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="G11" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" s="51">
         <v>2002</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="51">
         <v>166</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="J11" s="51"/>
+    </row>
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="51">
         <v>2002</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="G12" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="51">
         <v>2002</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="51">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="J12" s="51"/>
+    </row>
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="51">
         <v>2002</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="G13" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="51">
         <v>2002</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="51">
         <v>349</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="J13" s="51"/>
+    </row>
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="51">
         <v>2003</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H14" s="1">
+      <c r="G14" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="51">
         <v>2003</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="51">
         <v>25481</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="J14" s="51"/>
+    </row>
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="51">
         <v>2003</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="G15" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="51">
         <v>2003</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="51">
         <v>2202</v>
       </c>
+      <c r="J15" s="51"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="A16" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="51">
         <v>2003</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H16" s="1">
+      <c r="G16" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="51">
         <v>2003</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="51">
         <v>172</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="J16" s="51"/>
+    </row>
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17" s="51">
         <v>2003</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="G17" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="51">
         <v>2003</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="51">
         <v>170</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="J17" s="51"/>
+    </row>
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" s="51">
         <v>2003</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="G18" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="51">
         <v>2003</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="51">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="J18" s="51"/>
+    </row>
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="51">
         <v>2003</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" s="1">
+      <c r="G19" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="51">
         <v>2003</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="51">
         <v>351</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="1">
+      <c r="J19" s="51"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="51">
         <v>1997</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H20" s="1">
+      <c r="G20" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" s="51">
         <v>1997</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="51">
         <v>28539</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C21" s="1">
+      <c r="J20" s="51"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="51">
         <v>2002</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H21" s="1">
+      <c r="G21" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" s="51">
         <v>2002</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21" s="51">
         <v>28397</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C22" s="1">
+      <c r="J21" s="51"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="51">
         <v>2003</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H22" s="1">
+      <c r="G22" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H22" s="51">
         <v>2003</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="51">
         <v>28390</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C23" s="1">
+      <c r="J22" s="51"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="51">
         <v>2007</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H23" s="1">
+      <c r="G23" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H23" s="51">
         <v>2006</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="51">
         <v>30189</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C24" s="1">
+      <c r="J23" s="51"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="51">
         <v>2011</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H24" s="1">
+      <c r="G24" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="51">
         <v>2010</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24" s="51">
         <v>30250</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="J24" s="51"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="G25" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" s="51">
         <v>2014</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="51">
         <v>30250</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="J25" s="51"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H26" s="1">
+      <c r="G26" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="51">
         <v>2015</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26" s="51">
         <v>30250</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="J26" s="51"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="G27" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" s="51">
         <v>2016</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27" s="51">
         <v>28171</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="J27" s="51"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H28" s="1">
+      <c r="G28" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H28" s="51">
         <v>2017</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28" s="51">
         <v>28171</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="J28" s="51"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H29" s="1">
+      <c r="G29" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="51">
         <v>2018</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29" s="51">
         <v>28171</v>
       </c>
+      <c r="J29" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -38748,8 +38938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -38836,23 +39026,20 @@
       <c r="F2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>3400000</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>1997</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>2017</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="M2" s="1">
         <v>100</v>
@@ -38867,6 +39054,9 @@
         <v>487</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>128</v>
       </c>
     </row>
@@ -38889,23 +39079,20 @@
       <c r="F3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>3250000</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>2002</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>2017</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="M3" s="1">
         <v>100</v>
@@ -38920,6 +39107,9 @@
         <v>487</v>
       </c>
       <c r="Q3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>128</v>
       </c>
     </row>
@@ -38942,23 +39132,20 @@
       <c r="F4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>11999417</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>2003</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>2020</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="M4" s="1">
         <v>100</v>
@@ -38973,6 +39160,9 @@
         <v>487</v>
       </c>
       <c r="Q4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>128</v>
       </c>
     </row>
@@ -38995,23 +39185,20 @@
       <c r="F5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>25000000</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>2007</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>2027</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="M5" s="1">
         <v>100</v>
@@ -39026,6 +39213,9 @@
         <v>487</v>
       </c>
       <c r="Q5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>128</v>
       </c>
     </row>
@@ -39048,23 +39238,20 @@
       <c r="F6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>50000000</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>2011</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>2036</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="M6" s="1">
         <v>110</v>
@@ -39079,6 +39266,9 @@
         <v>487</v>
       </c>
       <c r="Q6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>235</v>
       </c>
     </row>
@@ -39101,23 +39291,20 @@
       <c r="F7" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>25130000</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>2015</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>2027</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="M7" s="1">
         <v>110</v>
@@ -39132,6 +39319,9 @@
         <v>487</v>
       </c>
       <c r="Q7" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>335</v>
       </c>
       <c r="S7" s="1" t="s">
@@ -46675,7 +46865,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>